<commit_message>
Update xlsx and ppt
</commit_message>
<xml_diff>
--- a/other/Calculations.xlsx
+++ b/other/Calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uantwerpen-my.sharepoint.com/personal/s0220625_ad_ua_ac_be/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A0DF95EF-C8E4-499A-83CF-F07B1A311405}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CC464F7A-B46E-45F6-8E8F-953DDA02AD8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="10800" firstSheet="4" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="10800" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -229,7 +229,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="152">
   <si>
     <t>KOS Calculation</t>
   </si>
@@ -591,18 +591,18 @@
     <t>Given budget by: Chief Financial Officer: Lye G. Batenkaitos</t>
   </si>
   <si>
+    <t>Estimation costs</t>
+  </si>
+  <si>
+    <t>Cost per used part (dry)</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
     <t>Funds (F)</t>
   </si>
   <si>
-    <t>Estimation costs</t>
-  </si>
-  <si>
-    <t>Cost per used part</t>
-  </si>
-  <si>
-    <t>Category</t>
-  </si>
-  <si>
     <t>approximately usgae of funds</t>
   </si>
   <si>
@@ -621,83 +621,77 @@
     <t>Launch Vehicle</t>
   </si>
   <si>
+    <t>Transfer Stage</t>
+  </si>
+  <si>
+    <t>Contingency (15%)</t>
+  </si>
+  <si>
+    <t>Total Estimated Cost</t>
+  </si>
+  <si>
+    <t>actual costs parts</t>
+  </si>
+  <si>
+    <t>difference with estimation</t>
+  </si>
+  <si>
+    <t>total dry parts cost</t>
+  </si>
+  <si>
+    <t>Resources</t>
+  </si>
+  <si>
+    <t>Weight(kg)</t>
+  </si>
+  <si>
+    <t>price per kg (F/kg)</t>
+  </si>
+  <si>
+    <t>price (F)</t>
+  </si>
+  <si>
     <t>AE-FF2 Airstream Protective Shell (2,5m)</t>
   </si>
   <si>
-    <t>Transfer Stage</t>
-  </si>
-  <si>
-    <t>Contingency (10%)</t>
-  </si>
-  <si>
-    <t>Contingency (15%)</t>
+    <t>MonoPropolent</t>
+  </si>
+  <si>
+    <t>LiquidFuel</t>
   </si>
   <si>
     <t>CompoMax Radial Tubeless (kOS)</t>
   </si>
   <si>
-    <t>Total Estimated Cost</t>
-  </si>
-  <si>
-    <t>Leftover Cost</t>
-  </si>
-  <si>
-    <t>actual costs</t>
-  </si>
-  <si>
-    <t>difference with estimation</t>
-  </si>
-  <si>
-    <t>F/m^2</t>
-  </si>
-  <si>
-    <t>Resources</t>
-  </si>
-  <si>
-    <t>Weight(kg)</t>
-  </si>
-  <si>
-    <t>price per F/kg</t>
-  </si>
-  <si>
-    <t>price</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TT18-A Launch Stability Enhancer </t>
-  </si>
-  <si>
-    <t>MonoPropolent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LT-2 Landing Strut </t>
-  </si>
-  <si>
-    <t>LiquidFuel</t>
-  </si>
-  <si>
     <t>Oxidizer</t>
   </si>
   <si>
-    <t>F</t>
-  </si>
-  <si>
     <t>SolidFuel</t>
   </si>
   <si>
-    <t>budget leftover</t>
+    <t>total</t>
+  </si>
+  <si>
+    <t>what game says</t>
+  </si>
+  <si>
+    <t>diffrance</t>
+  </si>
+  <si>
+    <t>left over</t>
+  </si>
+  <si>
+    <t>Fairing Construction Estemate</t>
   </si>
   <si>
     <t>dry part total</t>
-  </si>
-  <si>
-    <t>total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -715,6 +709,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
@@ -739,7 +739,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -858,43 +858,6 @@
         <color rgb="FF000000"/>
       </left>
       <right/>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
       <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
@@ -970,13 +933,9 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
+      <left/>
       <right/>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
+      <top/>
       <bottom style="double">
         <color rgb="FF000000"/>
       </bottom>
@@ -985,24 +944,46 @@
     <border>
       <left/>
       <right/>
-      <top style="medium">
+      <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF000000"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top style="double">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right style="medium">
-        <color rgb="FF000000"/>
+      <right/>
+      <top style="double">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1"/>
       </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
+      <top style="double">
+        <color theme="1"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF000000"/>
+      <bottom style="thin">
+        <color theme="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1011,7 +992,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1029,11 +1010,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -1044,12 +1024,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyBorder="1"/>
@@ -1057,28 +1034,46 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1087,7 +1082,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1108,24 +1103,267 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="18">
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="medium">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="medium">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="double">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="medium">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="medium">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="double">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="double">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="double">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="double">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right/>
+        <top style="double">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="double">
+          <color theme="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -1163,7 +1401,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8CEA70F8-D9AD-4AF0-8B78-4D737E94B91D}" name="PartsList" displayName="PartsList" ref="A1:B35" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:B35" xr:uid="{8CEA70F8-D9AD-4AF0-8B78-4D737E94B91D}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{B5E39159-FEE8-4949-AC2C-EEBAC04FC5BC}" uniqueName="1" name="Name" queryTableFieldId="1" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{B5E39159-FEE8-4949-AC2C-EEBAC04FC5BC}" uniqueName="1" name="Name" queryTableFieldId="1" dataDxfId="17"/>
     <tableColumn id="2" xr3:uid="{26FFC319-9EFB-4FF7-8331-03670194021D}" uniqueName="2" name="Amount" queryTableFieldId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1171,21 +1409,49 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5AEC469C-ADBD-4430-AB23-4AB96A2EAE4C}" name="Table3" displayName="Table3" ref="N8:R43" totalsRowCount="1">
-  <autoFilter ref="N8:R42" xr:uid="{5AEC469C-ADBD-4430-AB23-4AB96A2EAE4C}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="N9:R42">
-    <sortCondition ref="N8:N42"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5AEC469C-ADBD-4430-AB23-4AB96A2EAE4C}" name="Table3" displayName="Table3" ref="H8:L42" totalsRowCount="1" totalsRowDxfId="16" totalsRowBorderDxfId="15">
+  <autoFilter ref="H8:L41" xr:uid="{5AEC469C-ADBD-4430-AB23-4AB96A2EAE4C}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="H9:L41">
+    <sortCondition ref="K8:K41"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{D79ED5F5-BB6C-4345-8A94-A45497493061}" name="Part"/>
-    <tableColumn id="2" xr3:uid="{9CBC8A00-8235-48A1-9ADF-8F55CF39CEA2}" name="Amount"/>
-    <tableColumn id="3" xr3:uid="{700221D6-552B-4BE0-9363-412742B1DDB8}" name="Cost"/>
-    <tableColumn id="4" xr3:uid="{B7A4AE4D-5908-4771-89B0-51900393DAD1}" name="Category" totalsRowLabel="dry part total"/>
-    <tableColumn id="5" xr3:uid="{80F77563-CDDC-43CA-9F47-F5F8AD567FE6}" name="Sub-total" totalsRowFunction="custom">
+    <tableColumn id="1" xr3:uid="{D79ED5F5-BB6C-4345-8A94-A45497493061}" name="Part" totalsRowDxfId="14" dataCellStyle="Hyperlink"/>
+    <tableColumn id="2" xr3:uid="{9CBC8A00-8235-48A1-9ADF-8F55CF39CEA2}" name="Amount" totalsRowDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{700221D6-552B-4BE0-9363-412742B1DDB8}" name="Cost" totalsRowDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{B7A4AE4D-5908-4771-89B0-51900393DAD1}" name="Category" totalsRowLabel="dry part total" totalsRowDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{80F77563-CDDC-43CA-9F47-F5F8AD567FE6}" name="Sub-total" totalsRowFunction="custom" totalsRowDxfId="10">
       <totalsRowFormula>SUM(Table3[Sub-total])</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7491FE3D-BAB3-4997-8FBC-65852819B0E8}" name="Tabel2" displayName="Tabel2" ref="A26:D31" totalsRowCount="1" headerRowDxfId="9" headerRowBorderDxfId="7" tableBorderDxfId="8">
+  <autoFilter ref="A26:D30" xr:uid="{7491FE3D-BAB3-4997-8FBC-65852819B0E8}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{E4A69D5C-4C62-4B9C-85EA-8967756702BB}" name="Resources"/>
+    <tableColumn id="2" xr3:uid="{6B10A319-0602-4419-BCCB-4A9736034182}" name="Weight(kg)"/>
+    <tableColumn id="3" xr3:uid="{D876EC2F-6C41-4F9C-AF40-7F50969A4603}" name="price per kg (F/kg)"/>
+    <tableColumn id="4" xr3:uid="{77F69493-680F-456A-A0DA-0EC511602A44}" name="price (F)" totalsRowFunction="custom" dataDxfId="5" totalsRowDxfId="6">
+      <calculatedColumnFormula>Tabel2[[#This Row],[price per kg (F/kg)]]*Tabel2[[#This Row],[Weight(kg)]]</calculatedColumnFormula>
+      <totalsRowFormula>SUM(D27:D30)</totalsRowFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E7450766-BD90-4D1B-AD53-33B804ECC5BD}" name="Tabel4" displayName="Tabel4" ref="A19:C24" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="2" tableBorderDxfId="3">
+  <autoFilter ref="A19:C24" xr:uid="{E7450766-BD90-4D1B-AD53-33B804ECC5BD}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{95075E94-A2BA-487D-B6D9-9A65C447209B}" name="Category"/>
+    <tableColumn id="2" xr3:uid="{E196C337-75D1-4B45-8EB4-99F90FCB527A}" name="Funds (F)" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{E960109B-825E-4E7B-A7E9-F62C6DEA9660}" name="difference with estimation" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1884,8 +2150,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="J43" sqref="J43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1935,30 +2201,30 @@
       <c r="D6" s="5"/>
     </row>
     <row r="9" spans="1:7" ht="14.25" customHeight="1">
-      <c r="A9" s="46" t="s">
+      <c r="A9" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="47"/>
-      <c r="C9" s="47"/>
-      <c r="D9" s="47"/>
-      <c r="E9" s="48"/>
+      <c r="B9" s="53"/>
+      <c r="C9" s="53"/>
+      <c r="D9" s="53"/>
+      <c r="E9" s="54"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="26" t="s">
+      <c r="A10" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="25" t="s">
+      <c r="B10" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="25" t="s">
+      <c r="C10" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="25" t="s">
+      <c r="D10" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="27" t="s">
+      <c r="E10" s="25" t="s">
         <v>12</v>
       </c>
       <c r="F10" s="3"/>
@@ -2014,7 +2280,7 @@
       <c r="E14" s="11"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="28" t="s">
+      <c r="A15" s="26" t="s">
         <v>36</v>
       </c>
       <c r="B15">
@@ -2027,7 +2293,7 @@
       <c r="E15" s="11"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="27" t="s">
         <v>36</v>
       </c>
       <c r="B16" s="13">
@@ -2041,13 +2307,13 @@
       <c r="E16" s="14"/>
     </row>
     <row r="19" spans="1:7" ht="14.25" customHeight="1">
-      <c r="A19" s="43" t="s">
+      <c r="A19" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="44"/>
-      <c r="C19" s="44"/>
-      <c r="D19" s="44"/>
-      <c r="E19" s="45"/>
+      <c r="B19" s="50"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="50"/>
+      <c r="E19" s="51"/>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="15" t="s">
@@ -2099,22 +2365,22 @@
       </c>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="42"/>
-      <c r="B26" s="42"/>
-      <c r="C26" s="42"/>
-      <c r="D26" s="42"/>
-      <c r="E26" s="42"/>
+      <c r="A26" s="48"/>
+      <c r="B26" s="48"/>
+      <c r="C26" s="48"/>
+      <c r="D26" s="48"/>
+      <c r="E26" s="48"/>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="32" t="s">
+      <c r="A27" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="B27" s="33"/>
-      <c r="C27" s="33"/>
-      <c r="D27" s="33"/>
-      <c r="E27" s="33"/>
-      <c r="F27" s="33"/>
-      <c r="G27" s="34"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="32"/>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="15" t="s">
@@ -2132,13 +2398,13 @@
       <c r="E28" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="F28" s="35"/>
-      <c r="G28" s="36" t="s">
+      <c r="F28" s="33"/>
+      <c r="G28" s="34" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="30" t="s">
+      <c r="A29" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B29">
@@ -2161,7 +2427,7 @@
       </c>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="30" t="s">
+      <c r="A30" s="28" t="s">
         <v>47</v>
       </c>
       <c r="B30">
@@ -2184,7 +2450,7 @@
       </c>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="30" t="s">
+      <c r="A31" s="28" t="s">
         <v>48</v>
       </c>
       <c r="B31">
@@ -2207,7 +2473,7 @@
       </c>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="31" t="s">
+      <c r="A32" s="29" t="s">
         <v>49</v>
       </c>
       <c r="B32" s="13">
@@ -2242,7 +2508,7 @@
       </c>
     </row>
     <row r="39" spans="1:7">
-      <c r="A39" s="30" t="s">
+      <c r="A39" s="28" t="s">
         <v>51</v>
       </c>
       <c r="B39">
@@ -2265,7 +2531,7 @@
       </c>
     </row>
     <row r="40" spans="1:7">
-      <c r="A40" s="30" t="s">
+      <c r="A40" s="28" t="s">
         <v>52</v>
       </c>
       <c r="B40">
@@ -2323,21 +2589,21 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:20">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="55" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="N2" s="50" t="s">
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="N2" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="O2" s="50"/>
-      <c r="P2" s="50"/>
-      <c r="Q2" s="50"/>
-      <c r="R2" s="50"/>
-      <c r="S2" s="50"/>
-      <c r="T2" s="50"/>
+      <c r="O2" s="56"/>
+      <c r="P2" s="56"/>
+      <c r="Q2" s="56"/>
+      <c r="R2" s="56"/>
+      <c r="S2" s="56"/>
+      <c r="T2" s="56"/>
     </row>
     <row r="3" spans="1:20">
       <c r="A3" s="3" t="s">
@@ -2826,28 +3092,34 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FC5B483-7FF1-4686-A0C5-A1F86516AE53}">
-  <dimension ref="A1:V45"/>
+  <dimension ref="A1:O42"/>
   <sheetViews>
-    <sheetView topLeftCell="I4" workbookViewId="0">
-      <selection activeCell="N30" sqref="N30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="33.85546875" customWidth="1"/>
-    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" customWidth="1"/>
     <col min="3" max="3" width="31.28515625" customWidth="1"/>
     <col min="4" max="4" width="18.140625" customWidth="1"/>
     <col min="8" max="8" width="35.42578125" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" customWidth="1"/>
-    <col min="11" max="11" width="34" customWidth="1"/>
-    <col min="14" max="14" width="45" customWidth="1"/>
-    <col min="15" max="15" width="10.28515625" customWidth="1"/>
+    <col min="9" max="9" width="5.5703125" customWidth="1"/>
+    <col min="11" max="11" width="18.28515625" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" customWidth="1"/>
+    <col min="13" max="13" width="15.7109375" customWidth="1"/>
+    <col min="14" max="14" width="16.140625" customWidth="1"/>
+    <col min="15" max="15" width="20.85546875" customWidth="1"/>
+    <col min="16" max="16" width="11" customWidth="1"/>
     <col min="17" max="17" width="23.140625" customWidth="1"/>
     <col min="18" max="18" width="11.28515625" customWidth="1"/>
+    <col min="19" max="19" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.42578125" customWidth="1"/>
+    <col min="21" max="21" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:15">
       <c r="N1" s="3" t="s">
         <v>117</v>
       </c>
@@ -2855,140 +3127,99 @@
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
-      <c r="A2" s="53" t="s">
+    <row r="2" spans="1:15">
+      <c r="A2" s="59" t="s">
         <v>119</v>
       </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-    </row>
-    <row r="3" spans="1:18">
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3">
         <v>160000</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" s="57" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="7" spans="1:18">
-      <c r="A7" s="51" t="s">
+      <c r="B7" s="58"/>
+      <c r="D7" s="59"/>
+      <c r="E7" s="59"/>
+      <c r="H7" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="B7" s="52"/>
-      <c r="D7" s="53"/>
-      <c r="E7" s="53"/>
-      <c r="H7" s="18" t="s">
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="19"/>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="20"/>
-      <c r="N7" s="18" t="s">
+      <c r="B8" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="C8" s="35" t="s">
+        <v>124</v>
+      </c>
+      <c r="H8" t="s">
+        <v>125</v>
+      </c>
+      <c r="I8" t="s">
+        <v>84</v>
+      </c>
+      <c r="J8" t="s">
+        <v>126</v>
+      </c>
+      <c r="K8" t="s">
         <v>122</v>
       </c>
-      <c r="O7" s="19"/>
-      <c r="P7" s="19"/>
-      <c r="Q7" s="19"/>
-      <c r="R7" s="20"/>
-    </row>
-    <row r="8" spans="1:18">
-      <c r="A8" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="C8" s="37" t="s">
-        <v>124</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="I8" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="J8" s="17" t="s">
-        <v>126</v>
-      </c>
-      <c r="K8" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="L8" s="9" t="s">
+      <c r="L8" t="s">
         <v>127</v>
       </c>
-      <c r="N8" t="s">
-        <v>125</v>
-      </c>
-      <c r="O8" t="s">
-        <v>84</v>
-      </c>
-      <c r="P8" t="s">
-        <v>126</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>123</v>
-      </c>
-      <c r="R8" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18">
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="21">
+      <c r="B9" s="20">
         <v>45000</v>
       </c>
       <c r="C9">
         <v>0.3</v>
       </c>
-      <c r="H9" s="10" t="s">
-        <v>102</v>
+      <c r="H9" s="4" t="s">
+        <v>88</v>
       </c>
       <c r="I9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J9">
-        <v>3202</v>
+        <v>230</v>
       </c>
       <c r="K9" t="s">
         <v>15</v>
       </c>
-      <c r="L9" s="11">
-        <f t="shared" ref="L9:L14" si="0">I9*J9</f>
-        <v>9606</v>
-      </c>
-      <c r="N9" t="s">
-        <v>88</v>
-      </c>
-      <c r="O9">
-        <v>2</v>
-      </c>
-      <c r="P9">
-        <v>230</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>15</v>
-      </c>
-      <c r="R9">
-        <f>O9*P9</f>
+      <c r="L9">
+        <f>Table3[[#This Row],[Amount]]*Table3[[#This Row],[Cost]]</f>
         <v>460</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:15">
       <c r="A10" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="B10" s="21">
+      <c r="B10" s="20">
         <v>12000</v>
       </c>
       <c r="C10">
         <v>0.1</v>
       </c>
-      <c r="H10" s="10" t="s">
+      <c r="H10" s="4" t="s">
         <v>103</v>
       </c>
       <c r="I10">
@@ -2997,1299 +3228,842 @@
       <c r="J10">
         <v>300</v>
       </c>
-      <c r="K10" t="s">
+      <c r="K10" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="L10" s="11">
-        <f t="shared" si="0"/>
+      <c r="L10">
+        <f>Table3[[#This Row],[Amount]]*Table3[[#This Row],[Cost]]</f>
         <v>300</v>
       </c>
-      <c r="N10" t="s">
-        <v>109</v>
-      </c>
-      <c r="O10">
-        <v>3</v>
-      </c>
-      <c r="P10">
-        <v>240</v>
-      </c>
-      <c r="Q10" s="41" t="s">
-        <v>128</v>
-      </c>
-      <c r="R10">
-        <f>O10*P10</f>
-        <v>720</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18">
+    </row>
+    <row r="11" spans="1:15">
       <c r="A11" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="B11" s="22">
+      <c r="B11" s="21">
         <v>60000</v>
       </c>
       <c r="C11">
         <v>0.4</v>
       </c>
-      <c r="H11" s="10" t="s">
-        <v>86</v>
+      <c r="H11" s="4" t="s">
+        <v>101</v>
       </c>
       <c r="I11">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="J11">
-        <v>4500</v>
-      </c>
-      <c r="K11" t="s">
+        <v>340</v>
+      </c>
+      <c r="K11" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="L11" s="11">
-        <f t="shared" si="0"/>
-        <v>27000</v>
-      </c>
-      <c r="N11" t="s">
+      <c r="L11">
+        <f>Table3[[#This Row],[Amount]]*Table3[[#This Row],[Cost]]</f>
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="O11">
-        <v>1</v>
-      </c>
-      <c r="P11">
-        <v>600</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>128</v>
-      </c>
-      <c r="R11">
-        <f>O11*P11</f>
-        <v>600</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18">
-      <c r="A12" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="B12" s="22">
-        <v>15000</v>
+      <c r="B12" s="21">
+        <v>25000</v>
       </c>
       <c r="C12">
         <v>0.1</v>
       </c>
-      <c r="H12" s="10" t="s">
-        <v>48</v>
+      <c r="H12" s="4" t="s">
+        <v>102</v>
       </c>
       <c r="I12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J12">
-        <v>70</v>
-      </c>
-      <c r="K12" t="s">
+        <v>3202</v>
+      </c>
+      <c r="K12" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="L12" s="11">
-        <f t="shared" si="0"/>
-        <v>140</v>
-      </c>
-      <c r="N12" t="s">
-        <v>103</v>
-      </c>
-      <c r="O12">
-        <v>1</v>
-      </c>
-      <c r="P12">
-        <v>300</v>
-      </c>
-      <c r="Q12" s="41" t="s">
-        <v>15</v>
-      </c>
-      <c r="R12">
-        <f>O12*P12</f>
-        <v>300</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18">
+      <c r="L12">
+        <f>Table3[[#This Row],[Amount]]*Table3[[#This Row],[Cost]]</f>
+        <v>9606</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="B13" s="23">
-        <f>0.1*A3</f>
+        <v>131</v>
+      </c>
+      <c r="B13" s="22">
+        <f>A3*0.1</f>
         <v>16000</v>
       </c>
       <c r="C13">
         <v>0.1</v>
       </c>
-      <c r="H13" s="10" t="s">
-        <v>104</v>
+      <c r="H13" s="4" t="s">
+        <v>51</v>
       </c>
       <c r="I13">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="J13">
-        <v>16</v>
+        <v>1200</v>
       </c>
       <c r="K13" t="s">
-        <v>133</v>
-      </c>
-      <c r="L13" s="11">
-        <f t="shared" si="0"/>
-        <v>112</v>
-      </c>
-      <c r="N13" t="s">
-        <v>114</v>
-      </c>
-      <c r="O13">
-        <v>3</v>
-      </c>
-      <c r="P13">
-        <v>300</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>128</v>
-      </c>
-      <c r="R13">
-        <f>O13*P13</f>
-        <v>900</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18">
+        <v>15</v>
+      </c>
+      <c r="L13">
+        <f>Table3[[#This Row],[Amount]]*Table3[[#This Row],[Cost]]</f>
+        <v>4800</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" t="s">
+        <v>132</v>
+      </c>
+      <c r="B14">
+        <f>SUM(B9:B13)</f>
+        <v>158000</v>
+      </c>
       <c r="C14">
         <f>SUM(C9:C13)</f>
         <v>1</v>
       </c>
-      <c r="H14" s="10" t="s">
-        <v>105</v>
+      <c r="H14" s="4" t="s">
+        <v>87</v>
       </c>
       <c r="I14">
         <v>1</v>
       </c>
       <c r="J14">
-        <v>20</v>
+        <v>432.8</v>
       </c>
       <c r="K14" t="s">
+        <v>15</v>
+      </c>
+      <c r="L14">
+        <f>Table3[[#This Row],[Amount]]*Table3[[#This Row],[Cost]]</f>
+        <v>432.8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="H15" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="I15">
+        <v>6</v>
+      </c>
+      <c r="J15">
+        <v>4500</v>
+      </c>
+      <c r="K15" t="s">
+        <v>15</v>
+      </c>
+      <c r="L15">
+        <f>Table3[[#This Row],[Amount]]*Table3[[#This Row],[Cost]]</f>
+        <v>27000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="H16" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="I16">
+        <v>5</v>
+      </c>
+      <c r="J16">
+        <v>600</v>
+      </c>
+      <c r="K16" s="40" t="s">
+        <v>129</v>
+      </c>
+      <c r="L16">
+        <f>Table3[[#This Row],[Amount]]*Table3[[#This Row],[Cost]]</f>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="H17" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="I17">
+        <v>39</v>
+      </c>
+      <c r="J17">
+        <v>42</v>
+      </c>
+      <c r="K17" s="40" t="s">
+        <v>129</v>
+      </c>
+      <c r="L17">
+        <f>Table3[[#This Row],[Amount]]*Table3[[#This Row],[Cost]]</f>
+        <v>1638</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" s="36" t="s">
         <v>133</v>
       </c>
-      <c r="L14" s="11">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="N14" t="s">
+      <c r="B18" s="37"/>
+      <c r="C18" s="38"/>
+      <c r="H18" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="I18">
+        <v>2</v>
+      </c>
+      <c r="J18">
+        <v>450</v>
+      </c>
+      <c r="K18" s="40" t="s">
+        <v>129</v>
+      </c>
+      <c r="L18">
+        <f>Table3[[#This Row],[Amount]]*Table3[[#This Row],[Cost]]</f>
+        <v>900</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="C19" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="O14">
-        <v>4</v>
-      </c>
-      <c r="P14">
-        <v>2200</v>
-      </c>
-      <c r="Q14" s="41" t="s">
+      <c r="D19" s="3"/>
+      <c r="H19" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="J19">
+        <v>13000</v>
+      </c>
+      <c r="K19" t="s">
+        <v>129</v>
+      </c>
+      <c r="L19">
+        <f>Table3[[#This Row],[Amount]]*Table3[[#This Row],[Cost]]</f>
+        <v>13000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="6">
+        <f>SUMIF(
+    Table3[Category],
+    A20,
+    Table3[Sub-total])</f>
+        <v>43618.8</v>
+      </c>
+      <c r="C20" s="6">
+        <f>B9-B20</f>
+        <v>1381.1999999999971</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="J20">
+        <v>2812.4</v>
+      </c>
+      <c r="K20" t="s">
+        <v>129</v>
+      </c>
+      <c r="L20">
+        <f>Table3[[#This Row],[Amount]]*Table3[[#This Row],[Cost]]</f>
+        <v>2812.4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" t="s">
         <v>128</v>
       </c>
-      <c r="R14">
-        <f>O14*P14</f>
-        <v>8800</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18">
-      <c r="H15" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="I15">
-        <v>2.5</v>
-      </c>
-      <c r="J15">
-        <v>12</v>
-      </c>
-      <c r="K15" t="s">
-        <v>133</v>
-      </c>
-      <c r="L15" s="11">
-        <f>I15*J15+600</f>
-        <v>630</v>
-      </c>
-      <c r="N15" t="s">
-        <v>104</v>
-      </c>
-      <c r="O15">
-        <v>7</v>
-      </c>
-      <c r="P15">
-        <v>16</v>
-      </c>
-      <c r="Q15" s="41" t="s">
-        <v>128</v>
-      </c>
-      <c r="R15">
-        <f>O15*P15</f>
-        <v>112</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18">
-      <c r="H16" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="I16">
-        <v>4</v>
-      </c>
-      <c r="J16">
-        <v>300</v>
-      </c>
-      <c r="K16" t="s">
-        <v>133</v>
-      </c>
-      <c r="L16" s="11">
-        <f t="shared" ref="L16:L34" si="1">I16*J16</f>
-        <v>1200</v>
-      </c>
-      <c r="N16" t="s">
-        <v>94</v>
-      </c>
-      <c r="O16">
-        <v>5</v>
-      </c>
-      <c r="P16">
-        <v>600</v>
-      </c>
-      <c r="Q16" s="41" t="s">
+      <c r="B21" s="6">
+        <f>SUMIF(
+    Table3[Category],
+    A21,
+    Table3[Sub-total])</f>
+        <v>28916.92</v>
+      </c>
+      <c r="C21" s="6">
+        <f>B10-B21</f>
+        <v>-16916.919999999998</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="I21">
+        <v>2</v>
+      </c>
+      <c r="J21">
+        <v>1531.2</v>
+      </c>
+      <c r="K21" t="s">
         <v>129</v>
       </c>
-      <c r="R16">
-        <f>O16*P16</f>
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20">
-      <c r="A17" t="s">
+      <c r="L21">
+        <f>Table3[[#This Row],[Amount]]*Table3[[#This Row],[Cost]]</f>
+        <v>3062.4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" t="s">
+        <v>129</v>
+      </c>
+      <c r="B22" s="6">
+        <f>SUMIF(
+    Table3[Category],
+    A22,
+    Table3[Sub-total])</f>
+        <v>43532.800000000003</v>
+      </c>
+      <c r="C22" s="6">
+        <f>B11-B22</f>
+        <v>16467.199999999997</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="I22">
+        <v>2</v>
+      </c>
+      <c r="J22">
+        <v>8660</v>
+      </c>
+      <c r="K22" t="s">
+        <v>129</v>
+      </c>
+      <c r="L22">
+        <f>Table3[[#This Row],[Amount]]*Table3[[#This Row],[Cost]]</f>
+        <v>17320</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" t="s">
+        <v>130</v>
+      </c>
+      <c r="B23" s="6">
+        <f>SUMIF(
+    Table3[Category],
+    A23,
+    Table3[Sub-total])</f>
+        <v>6170</v>
+      </c>
+      <c r="C23" s="6">
+        <f>B12-B23</f>
+        <v>18830</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="I23">
+        <v>2</v>
+      </c>
+      <c r="J23">
+        <v>200</v>
+      </c>
+      <c r="K23" s="40" t="s">
+        <v>129</v>
+      </c>
+      <c r="L23">
+        <f>Table3[[#This Row],[Amount]]*Table3[[#This Row],[Cost]]</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" s="43" t="s">
         <v>135</v>
       </c>
-      <c r="B17">
-        <f>SUM(B9:B14)</f>
-        <v>148000</v>
-      </c>
-      <c r="H17" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="I17">
-        <v>3</v>
-      </c>
-      <c r="J17">
-        <v>150</v>
-      </c>
-      <c r="K17" t="s">
-        <v>133</v>
-      </c>
-      <c r="L17" s="11">
-        <f t="shared" si="1"/>
-        <v>450</v>
-      </c>
-      <c r="N17" t="s">
-        <v>99</v>
-      </c>
-      <c r="O17">
-        <v>39</v>
-      </c>
-      <c r="P17">
-        <v>42</v>
-      </c>
-      <c r="Q17" s="41" t="s">
+      <c r="B24" s="44">
+        <f>SUM(B20:B23)</f>
+        <v>122238.52</v>
+      </c>
+      <c r="C24" s="44"/>
+      <c r="H24" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="I24">
+        <v>2</v>
+      </c>
+      <c r="J24">
+        <v>700</v>
+      </c>
+      <c r="K24" t="s">
         <v>129</v>
       </c>
-      <c r="R17">
-        <f>O17*P17</f>
-        <v>1638</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20">
-      <c r="A18" t="s">
-        <v>136</v>
-      </c>
-      <c r="B18">
-        <f>A3-B17</f>
-        <v>12000</v>
-      </c>
-      <c r="H18" s="10" t="s">
+      <c r="L24">
+        <f>Table3[[#This Row],[Amount]]*Table3[[#This Row],[Cost]]</f>
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="H25" s="4" t="s">
         <v>109</v>
-      </c>
-      <c r="I18">
-        <v>3</v>
-      </c>
-      <c r="J18">
-        <v>240</v>
-      </c>
-      <c r="K18" t="s">
-        <v>131</v>
-      </c>
-      <c r="L18" s="11">
-        <f t="shared" si="1"/>
-        <v>720</v>
-      </c>
-      <c r="N18" t="s">
-        <v>101</v>
-      </c>
-      <c r="O18">
-        <v>3</v>
-      </c>
-      <c r="P18">
-        <v>340</v>
-      </c>
-      <c r="Q18" s="41" t="s">
-        <v>15</v>
-      </c>
-      <c r="R18">
-        <f>O18*P18</f>
-        <v>1020</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20">
-      <c r="H19" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="I19">
-        <v>3</v>
-      </c>
-      <c r="J19">
-        <v>70</v>
-      </c>
-      <c r="K19" t="s">
-        <v>128</v>
-      </c>
-      <c r="L19" s="11">
-        <f t="shared" si="1"/>
-        <v>210</v>
-      </c>
-      <c r="N19" t="s">
-        <v>102</v>
-      </c>
-      <c r="O19">
-        <v>3</v>
-      </c>
-      <c r="P19">
-        <v>3202</v>
-      </c>
-      <c r="Q19" s="41" t="s">
-        <v>15</v>
-      </c>
-      <c r="R19">
-        <f>O19*P19</f>
-        <v>9606</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20">
-      <c r="H20" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="I20">
-        <v>9</v>
-      </c>
-      <c r="J20">
-        <v>360</v>
-      </c>
-      <c r="K20" t="s">
-        <v>128</v>
-      </c>
-      <c r="L20" s="11">
-        <f t="shared" si="1"/>
-        <v>3240</v>
-      </c>
-      <c r="N20" t="s">
-        <v>95</v>
-      </c>
-      <c r="O20">
-        <v>2</v>
-      </c>
-      <c r="P20">
-        <v>820</v>
-      </c>
-      <c r="Q20" s="41" t="s">
-        <v>131</v>
-      </c>
-      <c r="R20">
-        <f>O20*P20</f>
-        <v>1640</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20">
-      <c r="H21" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="I21">
-        <v>6</v>
-      </c>
-      <c r="J21">
-        <v>380</v>
-      </c>
-      <c r="K21" t="s">
-        <v>128</v>
-      </c>
-      <c r="L21" s="11">
-        <f t="shared" si="1"/>
-        <v>2280</v>
-      </c>
-      <c r="N21" t="s">
-        <v>105</v>
-      </c>
-      <c r="O21">
-        <v>1</v>
-      </c>
-      <c r="P21">
-        <v>20</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>128</v>
-      </c>
-      <c r="R21">
-        <f>O21*P21</f>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20">
-      <c r="H22" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="I22">
-        <v>3</v>
-      </c>
-      <c r="J22">
-        <v>600</v>
-      </c>
-      <c r="K22" t="s">
-        <v>128</v>
-      </c>
-      <c r="L22" s="11">
-        <f t="shared" si="1"/>
-        <v>1800</v>
-      </c>
-      <c r="N22" t="s">
-        <v>110</v>
-      </c>
-      <c r="O22">
-        <v>3</v>
-      </c>
-      <c r="P22">
-        <v>51.64</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>128</v>
-      </c>
-      <c r="R22">
-        <f>O22*P22</f>
-        <v>154.92000000000002</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20">
-      <c r="H23" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="I23">
-        <v>3</v>
-      </c>
-      <c r="J23">
-        <v>300</v>
-      </c>
-      <c r="K23" t="s">
-        <v>128</v>
-      </c>
-      <c r="L23" s="11">
-        <f t="shared" si="1"/>
-        <v>900</v>
-      </c>
-      <c r="N23" t="s">
-        <v>51</v>
-      </c>
-      <c r="O23">
-        <v>4</v>
-      </c>
-      <c r="P23">
-        <v>1200</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>15</v>
-      </c>
-      <c r="R23">
-        <f>Table3[[#This Row],[Amount]]*Table3[[#This Row],[Cost]]</f>
-        <v>4800</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20">
-      <c r="H24" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="I24">
-        <v>3</v>
-      </c>
-      <c r="J24">
-        <v>1480</v>
-      </c>
-      <c r="K24" t="s">
-        <v>128</v>
-      </c>
-      <c r="L24" s="11">
-        <f t="shared" si="1"/>
-        <v>4440</v>
-      </c>
-      <c r="N24" t="s">
-        <v>112</v>
-      </c>
-      <c r="O24">
-        <v>6</v>
-      </c>
-      <c r="P24">
-        <v>380</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>128</v>
-      </c>
-      <c r="R24">
-        <f>O24*P24</f>
-        <v>2280</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20">
-      <c r="H25" s="10" t="s">
-        <v>116</v>
       </c>
       <c r="I25">
         <v>3</v>
       </c>
       <c r="J25">
-        <v>1800</v>
-      </c>
-      <c r="K25" t="s">
+        <v>240</v>
+      </c>
+      <c r="K25" s="40" t="s">
         <v>128</v>
       </c>
-      <c r="L25" s="11">
-        <f t="shared" si="1"/>
-        <v>5400</v>
-      </c>
-      <c r="N25" t="s">
-        <v>115</v>
-      </c>
-      <c r="O25">
+      <c r="L25">
+        <f>Table3[[#This Row],[Amount]]*Table3[[#This Row],[Cost]]</f>
+        <v>720</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" s="42" t="s">
+        <v>136</v>
+      </c>
+      <c r="B26" s="42" t="s">
+        <v>137</v>
+      </c>
+      <c r="C26" s="42" t="s">
+        <v>138</v>
+      </c>
+      <c r="D26" s="42" t="s">
+        <v>139</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="I26">
+        <v>1</v>
+      </c>
+      <c r="J26">
+        <v>600</v>
+      </c>
+      <c r="K26" t="s">
+        <v>128</v>
+      </c>
+      <c r="L26">
+        <f>Table3[[#This Row],[Amount]]*Table3[[#This Row],[Cost]]</f>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" t="s">
+        <v>141</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0.3</v>
+      </c>
+      <c r="D27">
+        <f>Tabel2[[#This Row],[price per kg (F/kg)]]*Tabel2[[#This Row],[Weight(kg)]]</f>
+        <v>0</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="I27">
         <v>3</v>
-      </c>
-      <c r="P25">
-        <v>1480</v>
-      </c>
-      <c r="Q25" t="s">
-        <v>128</v>
-      </c>
-      <c r="R25">
-        <f>O25*P25</f>
-        <v>4440</v>
-      </c>
-    </row>
-    <row r="26" spans="1:20">
-      <c r="H26" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="I26">
-        <v>2</v>
-      </c>
-      <c r="J26">
-        <v>230</v>
-      </c>
-      <c r="K26" t="s">
-        <v>131</v>
-      </c>
-      <c r="L26" s="11">
-        <f t="shared" si="1"/>
-        <v>460</v>
-      </c>
-      <c r="N26" t="s">
-        <v>98</v>
-      </c>
-      <c r="O26">
-        <v>2</v>
-      </c>
-      <c r="P26">
-        <v>450</v>
-      </c>
-      <c r="Q26" s="41" t="s">
-        <v>129</v>
-      </c>
-      <c r="R26">
-        <f>O26*P26</f>
-        <v>900</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20">
-      <c r="H27" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="I27">
-        <v>1</v>
       </c>
       <c r="J27">
         <v>300</v>
       </c>
       <c r="K27" t="s">
-        <v>131</v>
-      </c>
-      <c r="L27" s="11">
-        <f t="shared" si="1"/>
-        <v>300</v>
-      </c>
-      <c r="N27" t="s">
+        <v>128</v>
+      </c>
+      <c r="L27">
+        <f>Table3[[#This Row],[Amount]]*Table3[[#This Row],[Cost]]</f>
+        <v>900</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28" t="s">
+        <v>142</v>
+      </c>
+      <c r="B28">
+        <v>30870</v>
+      </c>
+      <c r="C28">
+        <v>0.16</v>
+      </c>
+      <c r="D28">
+        <f>Tabel2[[#This Row],[price per kg (F/kg)]]*Tabel2[[#This Row],[Weight(kg)]]</f>
+        <v>4939.2</v>
+      </c>
+      <c r="H28" t="s">
+        <v>143</v>
+      </c>
+      <c r="I28">
+        <v>4</v>
+      </c>
+      <c r="J28">
+        <v>2200</v>
+      </c>
+      <c r="K28" s="40" t="s">
+        <v>128</v>
+      </c>
+      <c r="L28">
+        <f>Table3[[#This Row],[Amount]]*Table3[[#This Row],[Cost]]</f>
+        <v>8800</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" t="s">
+        <v>144</v>
+      </c>
+      <c r="B29">
+        <v>37730</v>
+      </c>
+      <c r="C29">
+        <v>0.04</v>
+      </c>
+      <c r="D29">
+        <f>Tabel2[[#This Row],[price per kg (F/kg)]]*Tabel2[[#This Row],[Weight(kg)]]</f>
+        <v>1509.2</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="I29">
+        <v>7</v>
+      </c>
+      <c r="J29">
+        <v>16</v>
+      </c>
+      <c r="K29" s="40" t="s">
+        <v>128</v>
+      </c>
+      <c r="L29">
+        <f>Table3[[#This Row],[Amount]]*Table3[[#This Row],[Cost]]</f>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30" t="s">
+        <v>145</v>
+      </c>
+      <c r="B30">
+        <v>246000</v>
+      </c>
+      <c r="C30">
+        <v>0.08</v>
+      </c>
+      <c r="D30">
+        <f>Tabel2[[#This Row],[price per kg (F/kg)]]*Tabel2[[#This Row],[Weight(kg)]]</f>
+        <v>19680</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="I30">
+        <v>1</v>
+      </c>
+      <c r="J30">
+        <v>20</v>
+      </c>
+      <c r="K30" t="s">
+        <v>128</v>
+      </c>
+      <c r="L30">
+        <f>Table3[[#This Row],[Amount]]*Table3[[#This Row],[Cost]]</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="D31">
+        <f>SUM(D27:D30)</f>
+        <v>26128.400000000001</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="I31">
+        <v>3</v>
+      </c>
+      <c r="J31">
+        <v>51.64</v>
+      </c>
+      <c r="K31" t="s">
+        <v>128</v>
+      </c>
+      <c r="L31">
+        <f>Table3[[#This Row],[Amount]]*Table3[[#This Row],[Cost]]</f>
+        <v>154.92000000000002</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="H32" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="I32">
+        <v>6</v>
+      </c>
+      <c r="J32">
+        <v>380</v>
+      </c>
+      <c r="K32" t="s">
+        <v>128</v>
+      </c>
+      <c r="L32">
+        <f>Table3[[#This Row],[Amount]]*Table3[[#This Row],[Cost]]</f>
+        <v>2280</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
+      <c r="H33" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="I33">
+        <v>3</v>
+      </c>
+      <c r="J33">
+        <v>1480</v>
+      </c>
+      <c r="K33" t="s">
+        <v>128</v>
+      </c>
+      <c r="L33">
+        <f>Table3[[#This Row],[Amount]]*Table3[[#This Row],[Cost]]</f>
+        <v>4440</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12">
+      <c r="A34" t="s">
+        <v>146</v>
+      </c>
+      <c r="B34">
+        <f>Table3[[#Totals],[Sub-total]]+D31</f>
+        <v>148366.92000000001</v>
+      </c>
+      <c r="H34" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="O27">
+      <c r="I34">
         <v>3</v>
       </c>
-      <c r="P27">
+      <c r="J34">
         <v>1800</v>
       </c>
-      <c r="Q27" t="s">
+      <c r="K34" t="s">
         <v>128</v>
       </c>
-      <c r="R27">
+      <c r="L34">
         <f>Table3[[#This Row],[Amount]]*Table3[[#This Row],[Cost]]</f>
         <v>5400</v>
       </c>
     </row>
-    <row r="28" spans="1:20">
-      <c r="A28" s="55" t="s">
-        <v>137</v>
-      </c>
-      <c r="B28" s="56"/>
-      <c r="C28" s="57"/>
-      <c r="H28" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="I28">
-        <v>2</v>
-      </c>
-      <c r="J28">
-        <v>3000</v>
-      </c>
-      <c r="K28" t="s">
-        <v>131</v>
-      </c>
-      <c r="L28" s="11">
-        <f t="shared" si="1"/>
-        <v>6000</v>
-      </c>
-      <c r="N28" t="s">
-        <v>85</v>
-      </c>
-      <c r="O28">
+    <row r="35" spans="1:12">
+      <c r="A35" t="s">
+        <v>147</v>
+      </c>
+      <c r="B35">
+        <v>148365</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="I35">
+        <v>3</v>
+      </c>
+      <c r="J35">
+        <v>600</v>
+      </c>
+      <c r="K35" t="s">
+        <v>128</v>
+      </c>
+      <c r="L35">
+        <f>Table3[[#This Row],[Amount]]*Table3[[#This Row],[Cost]]</f>
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
+      <c r="A36" s="41" t="s">
+        <v>148</v>
+      </c>
+      <c r="B36">
+        <f>B34-B35</f>
+        <v>1.9200000000128057</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="I36">
+        <v>3</v>
+      </c>
+      <c r="J36">
+        <v>150</v>
+      </c>
+      <c r="K36" t="s">
+        <v>128</v>
+      </c>
+      <c r="L36">
+        <f>Table3[[#This Row],[Amount]]*Table3[[#This Row],[Cost]]</f>
+        <v>450</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
+      <c r="E37" s="39"/>
+      <c r="H37" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="I37">
+        <v>9</v>
+      </c>
+      <c r="J37">
+        <v>360</v>
+      </c>
+      <c r="K37" t="s">
+        <v>128</v>
+      </c>
+      <c r="L37">
+        <f>Table3[[#This Row],[Amount]]*Table3[[#This Row],[Cost]]</f>
+        <v>3240</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12">
+      <c r="A38" t="s">
+        <v>149</v>
+      </c>
+      <c r="B38">
+        <f>B14-B34</f>
+        <v>9633.0799999999872</v>
+      </c>
+      <c r="H38" t="s">
+        <v>150</v>
+      </c>
+      <c r="I38">
         <v>1</v>
       </c>
-      <c r="P28">
-        <v>3400</v>
-      </c>
-      <c r="Q28" s="41" t="s">
-        <v>131</v>
-      </c>
-      <c r="R28">
-        <f>O28*P28</f>
-        <v>3400</v>
-      </c>
-    </row>
-    <row r="29" spans="1:20">
-      <c r="A29" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="C29" s="16" t="s">
-        <v>138</v>
-      </c>
-      <c r="D29" s="3"/>
-      <c r="H29" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="I29">
-        <v>1</v>
-      </c>
-      <c r="J29">
-        <v>400</v>
-      </c>
-      <c r="K29" t="s">
-        <v>131</v>
-      </c>
-      <c r="L29" s="11">
-        <f t="shared" si="1"/>
-        <v>400</v>
-      </c>
-      <c r="N29" t="s">
-        <v>93</v>
-      </c>
-      <c r="O29">
-        <v>1</v>
-      </c>
-      <c r="P29">
-        <v>13000</v>
-      </c>
-      <c r="Q29" t="s">
-        <v>129</v>
-      </c>
-      <c r="R29">
-        <f>O29*P29</f>
-        <v>13000</v>
-      </c>
-    </row>
-    <row r="30" spans="1:20">
-      <c r="A30" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B30" s="6">
-        <f>SUM(L9:L12)</f>
-        <v>37046</v>
-      </c>
-      <c r="C30" s="22">
-        <f>B9-B30</f>
-        <v>7954</v>
-      </c>
-      <c r="H30" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="I30">
-        <v>1</v>
-      </c>
-      <c r="J30">
-        <v>5750</v>
-      </c>
-      <c r="K30" t="s">
-        <v>129</v>
-      </c>
-      <c r="L30" s="11">
-        <f t="shared" si="1"/>
-        <v>5750</v>
-      </c>
-      <c r="N30" t="s">
-        <v>92</v>
-      </c>
-      <c r="O30">
-        <v>1</v>
-      </c>
-      <c r="P30">
-        <v>2812.4</v>
-      </c>
-      <c r="Q30" t="s">
-        <v>129</v>
-      </c>
-      <c r="R30">
-        <f>O30*P30</f>
-        <v>2812.4</v>
-      </c>
-      <c r="T30" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="31" spans="1:20">
-      <c r="A31" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="B31" s="6">
-        <f>SUM(L19:L25)</f>
-        <v>18270</v>
-      </c>
-      <c r="C31" s="22">
-        <f>B10-B31</f>
-        <v>-6270</v>
-      </c>
-      <c r="H31" s="10" t="s">
+      <c r="J38">
+        <v>530</v>
+      </c>
+      <c r="K38" s="40" t="s">
+        <v>130</v>
+      </c>
+      <c r="L38">
+        <f>Table3[[#This Row],[Amount]]*Table3[[#This Row],[Cost]]</f>
+        <v>530</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
+      <c r="H39" s="4" t="s">
         <v>95</v>
-      </c>
-      <c r="I31">
-        <v>2</v>
-      </c>
-      <c r="J31">
-        <v>820</v>
-      </c>
-      <c r="K31" t="s">
-        <v>129</v>
-      </c>
-      <c r="L31" s="11">
-        <f t="shared" si="1"/>
-        <v>1640</v>
-      </c>
-      <c r="N31" t="s">
-        <v>90</v>
-      </c>
-      <c r="O31">
-        <v>2</v>
-      </c>
-      <c r="P31">
-        <v>1531.2</v>
-      </c>
-      <c r="Q31" t="s">
-        <v>129</v>
-      </c>
-      <c r="R31">
-        <f>O31*P31</f>
-        <v>3062.4</v>
-      </c>
-      <c r="T31">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="32" spans="1:20">
-      <c r="A32" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="B32" s="6">
-        <f>SUM(L30:L31)+SUM(L33:L37)+L39</f>
-        <v>63090</v>
-      </c>
-      <c r="C32" s="22">
-        <f>B11-B32</f>
-        <v>-3090</v>
-      </c>
-      <c r="H32" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="I32">
-        <v>1</v>
-      </c>
-      <c r="J32">
-        <v>3400</v>
-      </c>
-      <c r="K32" t="s">
-        <v>131</v>
-      </c>
-      <c r="L32" s="11">
-        <f t="shared" si="1"/>
-        <v>3400</v>
-      </c>
-      <c r="N32" t="s">
-        <v>87</v>
-      </c>
-      <c r="O32">
-        <v>1</v>
-      </c>
-      <c r="P32">
-        <v>432.8</v>
-      </c>
-      <c r="R32">
-        <f>O32*P32</f>
-        <v>432.8</v>
-      </c>
-    </row>
-    <row r="33" spans="1:22">
-      <c r="A33" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="B33" s="6">
-        <f>SUM(L26:L29)+L18+L32+L40</f>
-        <v>12300</v>
-      </c>
-      <c r="C33" s="22">
-        <f>B12-B33</f>
-        <v>2700</v>
-      </c>
-      <c r="H33" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="I33">
-        <v>1</v>
-      </c>
-      <c r="J33">
-        <v>13000</v>
-      </c>
-      <c r="K33" t="s">
-        <v>129</v>
-      </c>
-      <c r="L33" s="11">
-        <f t="shared" si="1"/>
-        <v>13000</v>
-      </c>
-      <c r="N33" t="s">
-        <v>97</v>
-      </c>
-      <c r="O33">
-        <v>2</v>
-      </c>
-      <c r="P33">
-        <v>8660</v>
-      </c>
-      <c r="R33">
-        <f>O33*P33</f>
-        <v>17320</v>
-      </c>
-    </row>
-    <row r="34" spans="1:22">
-      <c r="A34" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="B34" s="24">
-        <f>SUM(L13:L17)+L38</f>
-        <v>4050</v>
-      </c>
-      <c r="C34" s="23">
-        <f>B13-B34</f>
-        <v>11950</v>
-      </c>
-      <c r="H34" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="I34">
-        <v>5</v>
-      </c>
-      <c r="J34">
-        <v>600</v>
-      </c>
-      <c r="K34" t="s">
-        <v>129</v>
-      </c>
-      <c r="L34" s="11">
-        <f t="shared" si="1"/>
-        <v>3000</v>
-      </c>
-      <c r="N34" t="s">
-        <v>113</v>
-      </c>
-      <c r="O34">
-        <v>3</v>
-      </c>
-      <c r="P34">
-        <v>600</v>
-      </c>
-      <c r="Q34" t="s">
-        <v>128</v>
-      </c>
-      <c r="R34">
-        <f>O34*P34</f>
-        <v>1800</v>
-      </c>
-    </row>
-    <row r="35" spans="1:22">
-      <c r="H35" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="I35">
-        <v>2</v>
-      </c>
-      <c r="J35">
-        <v>700</v>
-      </c>
-      <c r="K35" t="s">
-        <v>129</v>
-      </c>
-      <c r="L35" s="11">
-        <f t="shared" ref="L35:L40" si="2">I35*J35</f>
-        <v>1400</v>
-      </c>
-      <c r="N35" t="s">
-        <v>108</v>
-      </c>
-      <c r="O35">
-        <v>3</v>
-      </c>
-      <c r="P35">
-        <v>150</v>
-      </c>
-      <c r="Q35" t="s">
-        <v>128</v>
-      </c>
-      <c r="R35">
-        <f>O35*P35</f>
-        <v>450</v>
-      </c>
-    </row>
-    <row r="36" spans="1:22">
-      <c r="H36" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="I36">
-        <v>2</v>
-      </c>
-      <c r="J36">
-        <v>18500</v>
-      </c>
-      <c r="K36" t="s">
-        <v>129</v>
-      </c>
-      <c r="L36" s="11">
-        <f t="shared" si="2"/>
-        <v>37000</v>
-      </c>
-      <c r="N36" t="s">
-        <v>89</v>
-      </c>
-      <c r="O36">
-        <v>1</v>
-      </c>
-      <c r="P36">
-        <v>300</v>
-      </c>
-      <c r="R36">
-        <f>O36*P36</f>
-        <v>300</v>
-      </c>
-    </row>
-    <row r="37" spans="1:22">
-      <c r="A37" s="54"/>
-      <c r="B37" s="54"/>
-      <c r="C37" s="54"/>
-      <c r="D37" s="54"/>
-      <c r="E37" s="54"/>
-      <c r="H37" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="I37">
-        <v>2</v>
-      </c>
-      <c r="J37">
-        <v>450</v>
-      </c>
-      <c r="K37" t="s">
-        <v>129</v>
-      </c>
-      <c r="L37" s="11">
-        <f t="shared" si="2"/>
-        <v>900</v>
-      </c>
-      <c r="N37" t="s">
-        <v>91</v>
-      </c>
-      <c r="O37">
-        <v>1</v>
-      </c>
-      <c r="P37">
-        <v>400</v>
-      </c>
-      <c r="R37">
-        <f>O37*P37+600</f>
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="38" spans="1:22">
-      <c r="H38" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="I38">
-        <v>39</v>
-      </c>
-      <c r="J38">
-        <v>42</v>
-      </c>
-      <c r="K38" t="s">
-        <v>133</v>
-      </c>
-      <c r="L38" s="11">
-        <f t="shared" si="2"/>
-        <v>1638</v>
-      </c>
-      <c r="N38" t="s">
-        <v>100</v>
-      </c>
-      <c r="O38">
-        <v>2</v>
-      </c>
-      <c r="P38">
-        <v>200</v>
-      </c>
-      <c r="R38">
-        <f>O38*P38</f>
-        <v>400</v>
-      </c>
-      <c r="S38" s="38" t="s">
-        <v>140</v>
-      </c>
-      <c r="T38" s="39" t="s">
-        <v>141</v>
-      </c>
-      <c r="U38" s="39" t="s">
-        <v>142</v>
-      </c>
-      <c r="V38" s="40" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="39" spans="1:22">
-      <c r="H39" s="10" t="s">
-        <v>144</v>
       </c>
       <c r="I39">
         <v>2</v>
       </c>
       <c r="J39">
-        <v>200</v>
-      </c>
-      <c r="K39" t="s">
-        <v>129</v>
-      </c>
-      <c r="L39" s="11">
-        <f t="shared" si="2"/>
-        <v>400</v>
-      </c>
-      <c r="N39" t="s">
-        <v>96</v>
-      </c>
-      <c r="O39">
+        <v>820</v>
+      </c>
+      <c r="K39" s="40" t="s">
+        <v>130</v>
+      </c>
+      <c r="L39">
+        <f>Table3[[#This Row],[Amount]]*Table3[[#This Row],[Cost]]</f>
+        <v>1640</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12">
+      <c r="H40" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="I40">
+        <v>1</v>
+      </c>
+      <c r="J40">
+        <v>3400</v>
+      </c>
+      <c r="K40" s="40" t="s">
+        <v>130</v>
+      </c>
+      <c r="L40">
+        <f>Table3[[#This Row],[Amount]]*Table3[[#This Row],[Cost]]</f>
+        <v>3400</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12">
+      <c r="H41" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="I41">
         <v>2</v>
       </c>
-      <c r="P39">
-        <v>700</v>
-      </c>
-      <c r="R39">
-        <f>O39*P39</f>
-        <v>1400</v>
-      </c>
-      <c r="S39" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="T39">
-        <v>0</v>
-      </c>
-      <c r="U39">
-        <v>0.3</v>
-      </c>
-      <c r="V39" s="11">
-        <f>T39*U39</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:22">
-      <c r="H40" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="I40" s="13">
-        <v>3</v>
-      </c>
-      <c r="J40" s="13">
-        <v>340</v>
-      </c>
-      <c r="K40" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="L40" s="14">
-        <f t="shared" si="2"/>
-        <v>1020</v>
-      </c>
-      <c r="N40" t="s">
-        <v>111</v>
-      </c>
-      <c r="O40">
-        <v>9</v>
-      </c>
-      <c r="P40">
-        <v>360</v>
-      </c>
-      <c r="Q40" t="s">
-        <v>128</v>
-      </c>
-      <c r="R40">
-        <f>O40*P40</f>
-        <v>3240</v>
-      </c>
-      <c r="S40" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="T40">
-        <v>30870</v>
-      </c>
-      <c r="U40">
-        <v>0.16</v>
-      </c>
-      <c r="V40" s="11">
-        <f>T40*U40</f>
-        <v>4939.2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:22">
-      <c r="N41" t="s">
-        <v>86</v>
-      </c>
-      <c r="O41">
-        <v>6</v>
-      </c>
-      <c r="P41">
-        <v>4500</v>
-      </c>
-      <c r="R41">
-        <f>O41*P41</f>
-        <v>27000</v>
-      </c>
-      <c r="S41" s="10" t="s">
-        <v>148</v>
-      </c>
-      <c r="T41">
-        <v>37730</v>
-      </c>
-      <c r="U41">
-        <v>0.04</v>
-      </c>
-      <c r="V41" s="11">
-        <f>T41*U41</f>
-        <v>1509.2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:22">
-      <c r="H42" t="s">
-        <v>30</v>
-      </c>
-      <c r="I42">
-        <f>SUM(L9:L43) + V43</f>
-        <v>160884.4</v>
-      </c>
-      <c r="J42" t="s">
-        <v>149</v>
-      </c>
-      <c r="S42" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="T42" s="13">
-        <v>246000</v>
-      </c>
-      <c r="U42" s="13">
-        <v>0.08</v>
-      </c>
-      <c r="V42" s="14">
-        <f>T42*U42</f>
-        <v>19680</v>
-      </c>
-    </row>
-    <row r="43" spans="1:22">
-      <c r="H43" t="s">
+      <c r="J41">
+        <v>300</v>
+      </c>
+      <c r="K41" t="s">
+        <v>130</v>
+      </c>
+      <c r="L41">
+        <f>Table3[[#This Row],[Amount]]*Table3[[#This Row],[Cost]]</f>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12">
+      <c r="H42" s="45"/>
+      <c r="I42" s="46"/>
+      <c r="J42" s="46"/>
+      <c r="K42" s="46" t="s">
         <v>151</v>
       </c>
-      <c r="I43">
-        <f>A3-I42</f>
-        <v>-884.39999999999418</v>
-      </c>
-      <c r="J43" t="s">
-        <v>149</v>
-      </c>
-      <c r="Q43" t="s">
-        <v>152</v>
-      </c>
-      <c r="R43">
+      <c r="L42" s="47">
         <f>SUM(Table3[Sub-total])</f>
-        <v>122408.51999999999</v>
-      </c>
-      <c r="V43">
-        <f>SUM(V39:V42)</f>
-        <v>26128.400000000001</v>
-      </c>
-    </row>
-    <row r="44" spans="1:22">
-      <c r="O44">
-        <f>SUM(Table3[Amount])</f>
-        <v>130</v>
-      </c>
-    </row>
-    <row r="45" spans="1:22">
-      <c r="Q45" t="s">
-        <v>153</v>
-      </c>
-      <c r="R45">
-        <f>Table3[[#Totals],[Sub-total]]+V43</f>
-        <v>148536.91999999998</v>
+        <v>122238.52</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="3">
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="D7:E7"/>
-    <mergeCell ref="A37:E37"/>
-    <mergeCell ref="A28:C28"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="H15" r:id="rId1" xr:uid="{5B12192D-0C11-41F7-98F5-4D626B56A05A}"/>
+    <hyperlink ref="H37" r:id="rId2" xr:uid="{2495BE1E-AEA5-4172-AF58-1BE05E6DAED3}"/>
+    <hyperlink ref="H24" r:id="rId3" xr:uid="{AA710EF4-08C3-437F-89C4-CC012E360F1F}"/>
+    <hyperlink ref="H23" r:id="rId4" xr:uid="{FA8683E5-2168-4D2D-9617-B5BE3677313A}"/>
+    <hyperlink ref="H41" r:id="rId5" xr:uid="{07FDC18A-6E28-4225-907F-6AC5794FFC02}"/>
+    <hyperlink ref="H36" r:id="rId6" xr:uid="{4BE51A23-A1D6-428D-91B4-15ADD247C561}"/>
+    <hyperlink ref="H35" r:id="rId7" xr:uid="{5E9E7584-8E0B-4C07-A666-6FCFCE2820D4}"/>
+    <hyperlink ref="H22" r:id="rId8" xr:uid="{3B02F796-4F45-4389-A5AD-C679FB2A8CEE}"/>
+    <hyperlink ref="H14" r:id="rId9" xr:uid="{05102AAB-EEAE-4BAB-BBFF-FCFA8B774546}"/>
+    <hyperlink ref="H21" r:id="rId10" xr:uid="{DEAEC810-2A4F-4E56-87F2-6FB67EEDB807}"/>
+    <hyperlink ref="H20" r:id="rId11" xr:uid="{59769B79-4C82-4012-AE1F-6389EDBED93B}"/>
+    <hyperlink ref="H19" r:id="rId12" xr:uid="{680A91B0-D05C-4863-8290-D49346C13ED5}"/>
+    <hyperlink ref="H40" r:id="rId13" xr:uid="{74347D53-1C1B-4E9D-A009-35F985056722}"/>
+    <hyperlink ref="H34" r:id="rId14" xr:uid="{4A17FDEF-F300-4A9C-B065-B0EB798F51E6}"/>
+    <hyperlink ref="H18" r:id="rId15" xr:uid="{38A95141-F343-4472-8DDB-80842C5CB99D}"/>
+    <hyperlink ref="H33" r:id="rId16" xr:uid="{0E77EDCD-F0EF-40EE-B028-25C2AAA8D2C0}"/>
+    <hyperlink ref="H32" r:id="rId17" xr:uid="{BAA581AB-F2D0-4050-96A3-86183550E2BB}"/>
+    <hyperlink ref="H13" r:id="rId18" xr:uid="{35B86F79-C812-49F8-99DE-88049905E82F}"/>
+    <hyperlink ref="H31" r:id="rId19" xr:uid="{09F365C3-92F7-49BD-BB0E-D1401F4E5C4D}"/>
+    <hyperlink ref="H30" r:id="rId20" xr:uid="{58BCD779-6709-434C-88C5-B5A2A9CE0867}"/>
+    <hyperlink ref="H39" r:id="rId21" xr:uid="{CB585EC0-BDAD-4AF8-B34F-D1D1FACCFDD2}"/>
+    <hyperlink ref="H12" r:id="rId22" xr:uid="{8B7B7737-CFB8-4697-B22C-5A3E98162C2D}"/>
+    <hyperlink ref="H11" r:id="rId23" xr:uid="{E7811A37-7635-4E85-87C8-05F6581B271A}"/>
+    <hyperlink ref="H17" r:id="rId24" xr:uid="{157A1AE4-4FDF-40DB-B79B-579603C9FBD2}"/>
+    <hyperlink ref="H16" r:id="rId25" xr:uid="{DEFA2427-E0B8-40A7-8A05-D9F3A4B7658D}"/>
+    <hyperlink ref="H29" r:id="rId26" xr:uid="{3CA5A058-73FB-4BC5-821B-1B748203325A}"/>
+    <hyperlink ref="H27" r:id="rId27" xr:uid="{31DE51EF-1B1C-47C2-B861-8253812199E1}"/>
+    <hyperlink ref="H10" r:id="rId28" xr:uid="{4244D169-A722-4AD4-811A-DF1764122AB6}"/>
+    <hyperlink ref="H26" r:id="rId29" xr:uid="{11214E08-945B-49A2-B79D-AFA6BB862C19}"/>
+    <hyperlink ref="H25" r:id="rId30" xr:uid="{0F864FC8-0D4E-4CC3-B6A8-0BFD22CE23C7}"/>
+    <hyperlink ref="H9" r:id="rId31" xr:uid="{3190AA09-876D-43F1-9EB3-153B96960FD2}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
+  <tableParts count="3">
+    <tablePart r:id="rId32"/>
+    <tablePart r:id="rId33"/>
+    <tablePart r:id="rId34"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>